<commit_message>
updating default category encoder to include delimiter
</commit_message>
<xml_diff>
--- a/resources/basic_schema_for_institutional_account_upload.xlsx
+++ b/resources/basic_schema_for_institutional_account_upload.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">http://www.solasistim.net/</t>
   </si>
   <si>
-    <t xml:space="preserve">Computer Software</t>
+    <t xml:space="preserve">Computer Software, Biochemistry</t>
   </si>
   <si>
     <t xml:space="preserve">David Banks</t>
@@ -193,17 +193,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.59"/>
@@ -214,7 +214,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="9.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
only print selectable categories
</commit_message>
<xml_diff>
--- a/resources/basic_schema_for_institutional_account_upload.xlsx
+++ b/resources/basic_schema_for_institutional_account_upload.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">http://www.solasistim.net/</t>
   </si>
   <si>
-    <t xml:space="preserve">Computer Software, Biochemistry</t>
+    <t xml:space="preserve">Networking and communications, Digital curation and preservation</t>
   </si>
   <si>
     <t xml:space="preserve">David Banks</t>
@@ -203,7 +203,7 @@
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.59"/>

</xml_diff>